<commit_message>
Fixed bug in initialization of first port
- All tests completed
</commit_message>
<xml_diff>
--- a/Testdoc.xlsx
+++ b/Testdoc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projekte\Lichtpult\Firmware\DMX_ArtNet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1F1D68-377B-4191-8604-1681C413D6D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D8184E-400A-489A-9ECC-13196C33C553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{EBF1B349-7774-48BC-8096-CDADDF09A2E0}"/>
   </bookViews>
@@ -218,16 +218,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -562,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66BC276-CF79-4493-BCEE-50BFDA5E687B}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -573,216 +570,225 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="7"/>
     </row>
     <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="8"/>
+      <c r="B16" s="7"/>
     </row>
     <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="8"/>
+      <c r="B17" s="7"/>
     </row>
     <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="8"/>
+      <c r="B18" s="7"/>
     </row>
     <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="8"/>
+      <c r="B19" s="7"/>
     </row>
     <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="8"/>
+      <c r="B20" s="7"/>
     </row>
     <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="8"/>
+      <c r="B21" s="7"/>
     </row>
     <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="8"/>
+      <c r="B22" s="7"/>
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="8"/>
+      <c r="B24" s="7"/>
     </row>
     <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="8"/>
+      <c r="B25" s="7"/>
     </row>
     <row r="26" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="8"/>
+      <c r="B26" s="7"/>
     </row>
     <row r="27" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="8"/>
+      <c r="B27" s="7"/>
     </row>
     <row r="28" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="8"/>
+      <c r="B28" s="7"/>
     </row>
     <row r="29" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
@@ -792,218 +798,227 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="6" t="s">
+      <c r="F29" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="8" t="s">
         <v>0</v>
       </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
     </row>
     <row r="32" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
     </row>
     <row r="33" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
     </row>
     <row r="36" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
     </row>
     <row r="37" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
     </row>
     <row r="39" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
     </row>
     <row r="40" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
     </row>
     <row r="41" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>12</v>
       </c>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
     </row>
     <row r="42" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
     </row>
     <row r="43" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="8"/>
+      <c r="B43" s="7"/>
     </row>
     <row r="44" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>15</v>
       </c>
-      <c r="B44" s="8"/>
+      <c r="B44" s="7"/>
     </row>
     <row r="45" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>16</v>
       </c>
-      <c r="B45" s="8"/>
+      <c r="B45" s="7"/>
     </row>
     <row r="46" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>17</v>
       </c>
-      <c r="B46" s="8"/>
+      <c r="B46" s="7"/>
     </row>
     <row r="47" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>18</v>
       </c>
-      <c r="B47" s="8"/>
+      <c r="B47" s="7"/>
     </row>
     <row r="48" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>19</v>
       </c>
-      <c r="B48" s="8"/>
+      <c r="B48" s="7"/>
     </row>
     <row r="49" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>20</v>
       </c>
-      <c r="B49" s="8"/>
+      <c r="B49" s="7"/>
     </row>
     <row r="50" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>21</v>
       </c>
-      <c r="B50" s="8"/>
+      <c r="B50" s="7"/>
     </row>
     <row r="51" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
     </row>
     <row r="52" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>23</v>
       </c>
-      <c r="B52" s="8"/>
+      <c r="B52" s="7"/>
     </row>
     <row r="53" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>24</v>
       </c>
-      <c r="B53" s="8"/>
+      <c r="B53" s="7"/>
     </row>
     <row r="54" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>25</v>
       </c>
-      <c r="B54" s="8"/>
+      <c r="B54" s="7"/>
     </row>
     <row r="55" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>26</v>
       </c>
-      <c r="B55" s="8"/>
+      <c r="B55" s="7"/>
     </row>
     <row r="56" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>29</v>
       </c>
-      <c r="B56" s="8"/>
+      <c r="B56" s="7"/>
     </row>
     <row r="57" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>39</v>
       </c>
-      <c r="B57" s="8"/>
+      <c r="B57" s="7"/>
     </row>
     <row r="58" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B58" s="2"/>
@@ -1016,43 +1031,63 @@
       <c r="A59" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B59" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
     </row>
     <row r="60" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>35</v>
       </c>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
     </row>
     <row r="61" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>31</v>
       </c>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
     </row>
     <row r="62" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>32</v>
       </c>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
     </row>
     <row r="63" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>33</v>
       </c>
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
     </row>
     <row r="64" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>34</v>
       </c>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
     </row>
     <row r="65" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>36</v>
       </c>
-      <c r="B65" s="8"/>
+      <c r="B65" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>